<commit_message>
Actualizacion - Semana 8
</commit_message>
<xml_diff>
--- a/DatosCacao_multivariado.xlsx
+++ b/DatosCacao_multivariado.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="n">
-        <v>6995.448154773418</v>
+        <v>4682.314840316323</v>
       </c>
     </row>
     <row r="3">
@@ -511,7 +511,7 @@
         <v>15859.11</v>
       </c>
       <c r="G3" t="n">
-        <v>6995.448154773418</v>
+        <v>4682.314840316323</v>
       </c>
     </row>
     <row r="4">
@@ -534,7 +534,7 @@
         <v>16854.62</v>
       </c>
       <c r="G4" t="n">
-        <v>6995.448154773418</v>
+        <v>4682.314840316323</v>
       </c>
     </row>
     <row r="5">
@@ -557,7 +557,7 @@
         <v>17707.29</v>
       </c>
       <c r="G5" t="n">
-        <v>6995.448154773418</v>
+        <v>4682.314840316323</v>
       </c>
     </row>
     <row r="6">
@@ -580,7 +580,7 @@
         <v>18378.07</v>
       </c>
       <c r="G6" t="n">
-        <v>6995.448154773418</v>
+        <v>4682.314840316323</v>
       </c>
     </row>
     <row r="7">
@@ -603,7 +603,7 @@
         <v>19995.38</v>
       </c>
       <c r="G7" t="n">
-        <v>5082.187533701564</v>
+        <v>5485.172645633665</v>
       </c>
     </row>
     <row r="8">
@@ -626,7 +626,7 @@
         <v>22029.23</v>
       </c>
       <c r="G8" t="n">
-        <v>5082.187533701564</v>
+        <v>5485.172645633665</v>
       </c>
     </row>
     <row r="9">
@@ -649,7 +649,7 @@
         <v>21029.01</v>
       </c>
       <c r="G9" t="n">
-        <v>5082.187533701564</v>
+        <v>5485.172645633665</v>
       </c>
     </row>
     <row r="10">
@@ -672,7 +672,7 @@
         <v>24491.28</v>
       </c>
       <c r="G10" t="n">
-        <v>5082.187533701564</v>
+        <v>5485.172645633665</v>
       </c>
     </row>
     <row r="11">
@@ -695,7 +695,7 @@
         <v>24283.07</v>
       </c>
       <c r="G11" t="n">
-        <v>4677.620854249429</v>
+        <v>4716.307814546833</v>
       </c>
     </row>
     <row r="12">
@@ -718,7 +718,7 @@
         <v>24571.8</v>
       </c>
       <c r="G12" t="n">
-        <v>4677.620854249429</v>
+        <v>4716.307814546833</v>
       </c>
     </row>
     <row r="13">
@@ -741,7 +741,7 @@
         <v>29584.14</v>
       </c>
       <c r="G13" t="n">
-        <v>4677.620854249429</v>
+        <v>4716.307814546833</v>
       </c>
     </row>
     <row r="14">
@@ -764,7 +764,7 @@
         <v>35211.13</v>
       </c>
       <c r="G14" t="n">
-        <v>4677.620854249429</v>
+        <v>4716.307814546833</v>
       </c>
     </row>
     <row r="15">
@@ -787,7 +787,7 @@
         <v>37151.2</v>
       </c>
       <c r="G15" t="n">
-        <v>5464.577071789913</v>
+        <v>6595.819040059065</v>
       </c>
     </row>
     <row r="16">
@@ -810,7 +810,7 @@
         <v>34765.19</v>
       </c>
       <c r="G16" t="n">
-        <v>5464.577071789913</v>
+        <v>6595.819040059065</v>
       </c>
     </row>
     <row r="17">
@@ -833,7 +833,7 @@
         <v>37710.51</v>
       </c>
       <c r="G17" t="n">
-        <v>5464.577071789913</v>
+        <v>6595.819040059065</v>
       </c>
     </row>
     <row r="18">
@@ -856,7 +856,7 @@
         <v>40459.25</v>
       </c>
       <c r="G18" t="n">
-        <v>5464.577071789913</v>
+        <v>6595.819040059065</v>
       </c>
     </row>
     <row r="19">
@@ -879,7 +879,7 @@
         <v>27858.69</v>
       </c>
       <c r="G19" t="n">
-        <v>7006.587945835642</v>
+        <v>4999.063386440928</v>
       </c>
     </row>
     <row r="20">
@@ -902,7 +902,7 @@
         <v>26162.48</v>
       </c>
       <c r="G20" t="n">
-        <v>7006.587945835642</v>
+        <v>4999.063386440928</v>
       </c>
     </row>
     <row r="21">
@@ -925,7 +925,7 @@
         <v>29338.3</v>
       </c>
       <c r="G21" t="n">
-        <v>7006.587945835642</v>
+        <v>4999.063386440928</v>
       </c>
     </row>
     <row r="22">
@@ -948,7 +948,7 @@
         <v>33858.99</v>
       </c>
       <c r="G22" t="n">
-        <v>6877.380492162348</v>
+        <v>7447.960279713438</v>
       </c>
     </row>
     <row r="23">
@@ -971,7 +971,7 @@
         <v>34249.61</v>
       </c>
       <c r="G23" t="n">
-        <v>6877.380492162348</v>
+        <v>7447.960279713438</v>
       </c>
     </row>
     <row r="24">
@@ -994,7 +994,7 @@
         <v>33644.16</v>
       </c>
       <c r="G24" t="n">
-        <v>6877.380492162348</v>
+        <v>7447.960279713438</v>
       </c>
     </row>
     <row r="25">
@@ -1017,7 +1017,7 @@
         <v>28626.19</v>
       </c>
       <c r="G25" t="n">
-        <v>6877.380492162348</v>
+        <v>7447.960279713438</v>
       </c>
     </row>
     <row r="26">
@@ -1040,7 +1040,7 @@
         <v>26420.24</v>
       </c>
       <c r="G26" t="n">
-        <v>5393.042676838491</v>
+        <v>5444.06118687639</v>
       </c>
     </row>
     <row r="27">
@@ -1063,7 +1063,7 @@
         <v>28459.54</v>
       </c>
       <c r="G27" t="n">
-        <v>5393.042676838491</v>
+        <v>5444.06118687639</v>
       </c>
     </row>
     <row r="28">
@@ -1086,7 +1086,7 @@
         <v>29856.83</v>
       </c>
       <c r="G28" t="n">
-        <v>5393.042676838491</v>
+        <v>5444.06118687639</v>
       </c>
     </row>
     <row r="29">
@@ -1109,7 +1109,7 @@
         <v>29783.02</v>
       </c>
       <c r="G29" t="n">
-        <v>5393.042676838491</v>
+        <v>5444.06118687639</v>
       </c>
     </row>
     <row r="30">
@@ -1132,7 +1132,7 @@
         <v>27632.22</v>
       </c>
       <c r="G30" t="n">
-        <v>5393.042676838491</v>
+        <v>5444.06118687639</v>
       </c>
     </row>
     <row r="31">
@@ -1155,7 +1155,7 @@
         <v>28260.15</v>
       </c>
       <c r="G31" t="n">
-        <v>3485.040500926388</v>
+        <v>4446.212064655101</v>
       </c>
     </row>
     <row r="32">
@@ -1178,7 +1178,7 @@
         <v>29589.63</v>
       </c>
       <c r="G32" t="n">
-        <v>3485.040500926388</v>
+        <v>4446.212064655101</v>
       </c>
     </row>
     <row r="33">
@@ -1201,7 +1201,7 @@
         <v>26306.81</v>
       </c>
       <c r="G33" t="n">
-        <v>3485.040500926388</v>
+        <v>4446.212064655101</v>
       </c>
     </row>
     <row r="34">
@@ -1224,7 +1224,7 @@
         <v>28690.57</v>
       </c>
       <c r="G34" t="n">
-        <v>3485.040500926388</v>
+        <v>4446.212064655101</v>
       </c>
     </row>
     <row r="35">
@@ -1247,7 +1247,7 @@
         <v>27399.09</v>
       </c>
       <c r="G35" t="n">
-        <v>2966.894382671454</v>
+        <v>3504.024688385195</v>
       </c>
     </row>
     <row r="36">
@@ -1270,7 +1270,7 @@
         <v>26987.45</v>
       </c>
       <c r="G36" t="n">
-        <v>2966.894382671454</v>
+        <v>3504.024688385195</v>
       </c>
     </row>
     <row r="37">
@@ -1293,7 +1293,7 @@
         <v>27345.52</v>
       </c>
       <c r="G37" t="n">
-        <v>2966.894382671454</v>
+        <v>3504.024688385195</v>
       </c>
     </row>
     <row r="38">
@@ -1316,7 +1316,7 @@
         <v>27873.32</v>
       </c>
       <c r="G38" t="n">
-        <v>2966.894382671454</v>
+        <v>3504.024688385195</v>
       </c>
     </row>
     <row r="39">
@@ -1339,7 +1339,7 @@
         <v>27937.68</v>
       </c>
       <c r="G39" t="n">
-        <v>2966.894382671454</v>
+        <v>3504.024688385195</v>
       </c>
     </row>
     <row r="40">
@@ -1362,7 +1362,7 @@
         <v>26031.12</v>
       </c>
       <c r="G40" t="n">
-        <v>4188.113109463453</v>
+        <v>5385.679067766575</v>
       </c>
     </row>
     <row r="41">
@@ -1385,7 +1385,7 @@
         <v>29345.11</v>
       </c>
       <c r="G41" t="n">
-        <v>4188.113109463453</v>
+        <v>5385.679067766575</v>
       </c>
     </row>
     <row r="42">
@@ -1408,7 +1408,7 @@
         <v>28748.79</v>
       </c>
       <c r="G42" t="n">
-        <v>4188.113109463453</v>
+        <v>5385.679067766575</v>
       </c>
     </row>
     <row r="43">
@@ -1431,7 +1431,7 @@
         <v>28035.74</v>
       </c>
       <c r="G43" t="n">
-        <v>4188.113109463453</v>
+        <v>5385.679067766575</v>
       </c>
     </row>
     <row r="44">
@@ -1454,7 +1454,7 @@
         <v>30793.52</v>
       </c>
       <c r="G44" t="n">
-        <v>6736.317447059654</v>
+        <v>7388.869513622338</v>
       </c>
     </row>
     <row r="45">
@@ -1477,7 +1477,7 @@
         <v>30897.78</v>
       </c>
       <c r="G45" t="n">
-        <v>6736.317447059654</v>
+        <v>7388.869513622338</v>
       </c>
     </row>
     <row r="46">
@@ -1500,7 +1500,7 @@
         <v>35039.04</v>
       </c>
       <c r="G46" t="n">
-        <v>6736.317447059654</v>
+        <v>7388.869513622338</v>
       </c>
     </row>
     <row r="47">
@@ -1523,7 +1523,7 @@
         <v>37979.15</v>
       </c>
       <c r="G47" t="n">
-        <v>6736.317447059654</v>
+        <v>7388.869513622338</v>
       </c>
     </row>
     <row r="48">
@@ -1546,7 +1546,7 @@
         <v>39496.42</v>
       </c>
       <c r="G48" t="n">
-        <v>8804.789830528243</v>
+        <v>7582.515471984145</v>
       </c>
     </row>
     <row r="49">
@@ -1569,7 +1569,7 @@
         <v>42514.35</v>
       </c>
       <c r="G49" t="n">
-        <v>8804.789830528243</v>
+        <v>7582.515471984145</v>
       </c>
     </row>
     <row r="50">
@@ -1592,7 +1592,7 @@
         <v>49217.54</v>
       </c>
       <c r="G50" t="n">
-        <v>8804.789830528243</v>
+        <v>7582.515471984145</v>
       </c>
     </row>
     <row r="51">
@@ -1615,7 +1615,7 @@
         <v>46319.09</v>
       </c>
       <c r="G51" t="n">
-        <v>8804.789830528243</v>
+        <v>7582.515471984145</v>
       </c>
     </row>
     <row r="52">
@@ -1638,7 +1638,7 @@
         <v>46450.08</v>
       </c>
       <c r="G52" t="n">
-        <v>6659.164709241046</v>
+        <v>9514.654555849344</v>
       </c>
     </row>
     <row r="53">
@@ -1661,7 +1661,7 @@
         <v>44801.56</v>
       </c>
       <c r="G53" t="n">
-        <v>6659.164709241046</v>
+        <v>9514.654555849344</v>
       </c>
     </row>
     <row r="54">
@@ -1684,7 +1684,7 @@
         <v>47574.84</v>
       </c>
       <c r="G54" t="n">
-        <v>6659.164709241046</v>
+        <v>9514.654555849344</v>
       </c>
     </row>
     <row r="55">
@@ -1707,7 +1707,7 @@
         <v>47202.56</v>
       </c>
       <c r="G55" t="n">
-        <v>6659.164709241046</v>
+        <v>9514.654555849344</v>
       </c>
     </row>
     <row r="56">
@@ -1730,7 +1730,7 @@
         <v>45175.27</v>
       </c>
       <c r="G56" t="n">
-        <v>4837.877877356153</v>
+        <v>5410.030976527181</v>
       </c>
     </row>
     <row r="57">
@@ -1753,7 +1753,7 @@
         <v>40040</v>
       </c>
       <c r="G57" t="n">
-        <v>4837.877877356153</v>
+        <v>5410.030976527181</v>
       </c>
     </row>
     <row r="58">
@@ -1776,7 +1776,7 @@
         <v>41858.18</v>
       </c>
       <c r="G58" t="n">
-        <v>4837.877877356153</v>
+        <v>5410.030976527181</v>
       </c>
     </row>
     <row r="59">
@@ -1799,7 +1799,7 @@
         <v>34057.69</v>
       </c>
       <c r="G59" t="n">
-        <v>4837.877877356153</v>
+        <v>5410.030976527181</v>
       </c>
     </row>
     <row r="60">
@@ -1822,7 +1822,7 @@
         <v>33237.68</v>
       </c>
       <c r="G60" t="n">
-        <v>4452.759426795676</v>
+        <v>4485.554779177548</v>
       </c>
     </row>
     <row r="61">
@@ -1845,7 +1845,7 @@
         <v>34334.11</v>
       </c>
       <c r="G61" t="n">
-        <v>4452.759426795676</v>
+        <v>4485.554779177548</v>
       </c>
     </row>
     <row r="62">
@@ -1868,7 +1868,7 @@
         <v>32132.11</v>
       </c>
       <c r="G62" t="n">
-        <v>4452.759426795676</v>
+        <v>4485.554779177548</v>
       </c>
     </row>
     <row r="63">
@@ -1891,7 +1891,7 @@
         <v>33443.65</v>
       </c>
       <c r="G63" t="n">
-        <v>4452.759426795676</v>
+        <v>4485.554779177548</v>
       </c>
     </row>
     <row r="64">
@@ -1914,7 +1914,7 @@
         <v>33199.58</v>
       </c>
       <c r="G64" t="n">
-        <v>4452.759426795676</v>
+        <v>4485.554779177548</v>
       </c>
     </row>
     <row r="65">
@@ -1937,7 +1937,7 @@
         <v>33932.93</v>
       </c>
       <c r="G65" t="n">
-        <v>5201.885280582115</v>
+        <v>3731.890260596616</v>
       </c>
     </row>
     <row r="66">
@@ -1960,7 +1960,7 @@
         <v>35304.14</v>
       </c>
       <c r="G66" t="n">
-        <v>5201.885280582115</v>
+        <v>3731.890260596616</v>
       </c>
     </row>
     <row r="67">
@@ -1983,7 +1983,7 @@
         <v>35963.92</v>
       </c>
       <c r="G67" t="n">
-        <v>5201.885280582115</v>
+        <v>3731.890260596616</v>
       </c>
     </row>
     <row r="68">
@@ -2006,7 +2006,7 @@
         <v>36278.43</v>
       </c>
       <c r="G68" t="n">
-        <v>5201.885280582115</v>
+        <v>3731.890260596616</v>
       </c>
     </row>
     <row r="69">
@@ -2029,7 +2029,7 @@
         <v>34509.18</v>
       </c>
       <c r="G69" t="n">
-        <v>6669.768991035239</v>
+        <v>6421.037168220616</v>
       </c>
     </row>
     <row r="70">
@@ -2052,7 +2052,7 @@
         <v>36788.04</v>
       </c>
       <c r="G70" t="n">
-        <v>6669.768991035239</v>
+        <v>6421.037168220616</v>
       </c>
     </row>
     <row r="71">
@@ -2075,7 +2075,7 @@
         <v>43378.63</v>
       </c>
       <c r="G71" t="n">
-        <v>6669.768991035239</v>
+        <v>6421.037168220616</v>
       </c>
     </row>
     <row r="72">
@@ -2098,7 +2098,7 @@
         <v>38907.27</v>
       </c>
       <c r="G72" t="n">
-        <v>6669.768991035239</v>
+        <v>6421.037168220616</v>
       </c>
     </row>
     <row r="73">
@@ -2121,7 +2121,7 @@
         <v>36656.72</v>
       </c>
       <c r="G73" t="n">
-        <v>6546.772765970662</v>
+        <v>6389.296100741921</v>
       </c>
     </row>
     <row r="74">
@@ -2144,7 +2144,7 @@
         <v>39371.64</v>
       </c>
       <c r="G74" t="n">
-        <v>6546.772765970662</v>
+        <v>6389.296100741921</v>
       </c>
     </row>
     <row r="75">
@@ -2167,7 +2167,7 @@
         <v>35596.62</v>
       </c>
       <c r="G75" t="n">
-        <v>6546.772765970662</v>
+        <v>6389.296100741921</v>
       </c>
     </row>
     <row r="76">
@@ -2190,7 +2190,7 @@
         <v>32538.48</v>
       </c>
       <c r="G76" t="n">
-        <v>6546.772765970662</v>
+        <v>6389.296100741921</v>
       </c>
     </row>
     <row r="77">
@@ -2213,7 +2213,7 @@
         <v>34094.35</v>
       </c>
       <c r="G77" t="n">
-        <v>6546.772765970662</v>
+        <v>6389.296100741921</v>
       </c>
     </row>
     <row r="78">
@@ -2236,7 +2236,7 @@
         <v>31159.06</v>
       </c>
       <c r="G78" t="n">
-        <v>5133.789669290597</v>
+        <v>4222.840907883964</v>
       </c>
     </row>
     <row r="79">
@@ -2259,7 +2259,7 @@
         <v>30820.7</v>
       </c>
       <c r="G79" t="n">
-        <v>5133.789669290597</v>
+        <v>4222.840907883964</v>
       </c>
     </row>
     <row r="80">
@@ -2282,7 +2282,7 @@
         <v>32259.05</v>
       </c>
       <c r="G80" t="n">
-        <v>5133.789669290597</v>
+        <v>4222.840907883964</v>
       </c>
     </row>
     <row r="81">
@@ -2305,7 +2305,7 @@
         <v>31543.28</v>
       </c>
       <c r="G81" t="n">
-        <v>3317.508499896306</v>
+        <v>3199.757991717083</v>
       </c>
     </row>
     <row r="82">
@@ -2328,7 +2328,7 @@
         <v>33768.07</v>
       </c>
       <c r="G82" t="n">
-        <v>3317.508499896306</v>
+        <v>3199.757991717083</v>
       </c>
     </row>
   </sheetData>

</xml_diff>